<commit_message>
Button method update (scroll)
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/LimitManagement.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/LimitManagement.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-922020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hbl-Automation-9102020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>limit_type</t>
   </si>
@@ -71,22 +71,10 @@
     <t>limit_name_tran_query</t>
   </si>
   <si>
-    <t>Funds Transfer to HBL Account</t>
-  </si>
-  <si>
-    <t>Utility Bills and Other Payments</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>Funds Transfer to Other Banks Account</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>23000</t>
+    <t>QR Payments</t>
+  </si>
+  <si>
+    <t>90000</t>
   </si>
 </sst>
 </file>
@@ -405,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,10 +443,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
@@ -476,64 +464,6 @@
         <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>